<commit_message>
fix: optimization for parentless nodes on cps-234
</commit_message>
<xml_diff>
--- a/tools/apra/cps-234.xlsx
+++ b/tools/apra/cps-234.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/apra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A62E48-DCA0-334C-9153-1DD585ADE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2868E8D-E5B9-2647-A7D3-CC5CEC51FB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="-28140" windowWidth="50880" windowHeight="27980" activeTab="1" xr2:uid="{BA5F8652-5CE3-1046-9B2F-E60A6A3155FF}"/>
+    <workbookView xWindow="4020" yWindow="-28140" windowWidth="50880" windowHeight="27980" xr2:uid="{BA5F8652-5CE3-1046-9B2F-E60A6A3155FF}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A32CF78-4899-844D-910E-C7C96DD50DBE}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView zoomScale="242" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="242" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,7 +684,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EB5204-7E14-174C-96A7-5A6105BDEBD6}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+    <sheetView zoomScale="138" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix convert_library to avoid such problems
</commit_message>
<xml_diff>
--- a/tools/apra/cps-234.xlsx
+++ b/tools/apra/cps-234.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/apra/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/apra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2868E8D-E5B9-2647-A7D3-CC5CEC51FB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93588C5E-B4A1-3144-8F37-B67D805FA89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="-28140" windowWidth="50880" windowHeight="27980" xr2:uid="{BA5F8652-5CE3-1046-9B2F-E60A6A3155FF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{BA5F8652-5CE3-1046-9B2F-E60A6A3155FF}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A32CF78-4899-844D-910E-C7C96DD50DBE}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="242" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="242" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EB5204-7E14-174C-96A7-5A6105BDEBD6}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0">
+    <sheetView zoomScale="258" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: optimization for parentless nodes on cps-234 (#1812)
* fix: optimization for parentless nodes on cps-234

* fix convert_library to avoid such problems

---------

Co-authored-by: eric-intuitem <71850047+eric-intuitem@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tools/apra/cps-234.xlsx
+++ b/tools/apra/cps-234.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/apra/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/apra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A62E48-DCA0-334C-9153-1DD585ADE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93588C5E-B4A1-3144-8F37-B67D805FA89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="-28140" windowWidth="50880" windowHeight="27980" activeTab="1" xr2:uid="{BA5F8652-5CE3-1046-9B2F-E60A6A3155FF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{BA5F8652-5CE3-1046-9B2F-E60A6A3155FF}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A32CF78-4899-844D-910E-C7C96DD50DBE}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView zoomScale="242" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="242" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,7 +684,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EB5204-7E14-174C-96A7-5A6105BDEBD6}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+    <sheetView zoomScale="258" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>